<commit_message>
run_program() name output files with ordinal number
</commit_message>
<xml_diff>
--- a/resource/test.xlsx
+++ b/resource/test.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mrowk\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mrowk\Nauka programowania\readingPDF\resource\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99D78CB6-BA12-431D-8A6A-3C13CDD0644A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9EB0A34-56D3-4195-B0AC-6AE34B8A9CD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2475" yWindow="915" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>NR faktury</t>
   </si>
@@ -70,6 +70,9 @@
   </si>
   <si>
     <t>Zamowienie-nr-8492.pdf</t>
+  </si>
+  <si>
+    <t>lp</t>
   </si>
 </sst>
 </file>
@@ -387,79 +390,100 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.140625" customWidth="1"/>
-    <col min="2" max="2" width="43.140625" customWidth="1"/>
+    <col min="2" max="2" width="24.140625" customWidth="1"/>
+    <col min="3" max="3" width="43.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
         <v>3</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
         <v>6</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
         <v>9</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
         <v>10</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
         <v>12</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B8">
         <v>8492</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>14</v>
       </c>
     </row>

</xml_diff>